<commit_message>
Added student name to pathways template;
</commit_message>
<xml_diff>
--- a/data/files/mschool_pathways_template.xlsx
+++ b/data/files/mschool_pathways_template.xlsx
@@ -19,38 +19,53 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Message</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Screen</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Pathway Date</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Student Id</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Order</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Url</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Student Name</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="4">
     <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <name val="Verdana"/>
     </font>
@@ -84,10 +99,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,47 +433,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="32.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="34.7109375" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="10.7109375" style="2"/>
+    <col min="1" max="1" width="12" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="32.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="34.7109375" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1"/>
       <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>

<commit_message>
updated pathway template columns;
</commit_message>
<xml_diff>
--- a/data/files/mschool_pathways_template.xlsx
+++ b/data/files/mschool_pathways_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="-20" windowWidth="24800" windowHeight="17260" tabRatio="500"/>
+    <workbookView xWindow="14320" yWindow="-80" windowWidth="14400" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,33 +19,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Message</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Screen</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Pathway Date</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Student Id</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Order</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Url</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Student Name</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resource</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Timer</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Student Number</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -53,12 +49,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
@@ -436,7 +426,7 @@
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -453,26 +443,24 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>

</xml_diff>

<commit_message>
Changed pathways table's 'order' column to 'step';
</commit_message>
<xml_diff>
--- a/data/files/mschool_pathways_template.xlsx
+++ b/data/files/mschool_pathways_template.xlsx
@@ -25,10 +25,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Order</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Student Name</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -42,6 +38,10 @@
   </si>
   <si>
     <t>Student Number</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Step</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -49,6 +49,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
@@ -426,7 +432,7 @@
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -443,22 +449,22 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>

</xml_diff>

<commit_message>
uploaded correct pathways template;
</commit_message>
<xml_diff>
--- a/data/files/mschool_pathways_template.xlsx
+++ b/data/files/mschool_pathways_template.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14320" yWindow="-80" windowWidth="14400" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="140" yWindow="-20" windowWidth="26120" windowHeight="11000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,30 +19,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Pathway Date</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Student Name</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Resource</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Timer</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Student Number</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Step</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Student ID</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>1st</t>
+  </si>
+  <si>
+    <t>2nd</t>
+  </si>
+  <si>
+    <t>3rd</t>
+  </si>
+  <si>
+    <t>4th</t>
+  </si>
+  <si>
+    <t>5th</t>
   </si>
 </sst>
 </file>
@@ -55,20 +58,36 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
-      <sz val="10"/>
-      <name val="Verdana"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Verdana"/>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Verdana"/>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue Light"/>
     </font>
     <font>
       <sz val="8"/>
@@ -92,16 +111,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -184,6 +205,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -218,6 +240,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -432,46 +455,46 @@
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="12" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="32.5703125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="34.7109375" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="10.7109375" style="2"/>
+    <col min="1" max="9" width="17.1640625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>